<commit_message>
Final dataset from CGM sensor test #2
</commit_message>
<xml_diff>
--- a/librelink/Rik Activity 2019.xlsx
+++ b/librelink/Rik Activity 2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc6084b92ffa451/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{A1AD52F5-5758-0A44-8A5A-0AE3A9C1C771}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{0A9802B7-B5C7-7743-ACE5-1C239ACC16D3}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="13_ncr:1_{A1AD52F5-5758-0A44-8A5A-0AE3A9C1C771}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{0E2459E2-D44D-664D-A164-4C905763F99B}"/>
   <bookViews>
-    <workbookView xWindow="21140" yWindow="3540" windowWidth="27640" windowHeight="16940" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
+    <workbookView xWindow="3100" yWindow="1100" windowWidth="27640" windowHeight="16940" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="126">
   <si>
     <t>Start</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Coffee w/ condensed milk (1TBS)</t>
   </si>
   <si>
-    <t>Pasta mushroom chicken</t>
-  </si>
-  <si>
     <t>Oatmeal w/butter</t>
   </si>
   <si>
@@ -358,6 +355,60 @@
   </si>
   <si>
     <t>CBD</t>
+  </si>
+  <si>
+    <t>Pork tamale</t>
+  </si>
+  <si>
+    <t>Coffee w/milk</t>
+  </si>
+  <si>
+    <t>Kombucha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food </t>
+  </si>
+  <si>
+    <t>Beans w/ham</t>
+  </si>
+  <si>
+    <t>Tofu and coconut rice</t>
+  </si>
+  <si>
+    <t>Grapefruit kefir smoothie</t>
+  </si>
+  <si>
+    <t>Royal milk tea</t>
+  </si>
+  <si>
+    <t>Pork loin, cabbage</t>
+  </si>
+  <si>
+    <t>Hamburger</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Coconut Shrimp and rice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fish + bread </t>
+  </si>
+  <si>
+    <t>Nuts</t>
+  </si>
+  <si>
+    <t>Pork loin</t>
+  </si>
+  <si>
+    <t>Pasta (chicken mushroom)</t>
+  </si>
+  <si>
+    <t>Beer (empty stomach)</t>
+  </si>
+  <si>
+    <t>Nuts + banana</t>
   </si>
 </sst>
 </file>
@@ -414,7 +465,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -481,6 +532,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -497,16 +579,57 @@
     <xf numFmtId="22" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yy\ h:mm"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="m/d/yy\ h:mm"/>
     </dxf>
@@ -524,10 +647,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:D107" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="A1:D107" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{378B7070-ADA2-F840-857A-A5C12E2181D6}" name="Start" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{50BA6A11-7F67-3245-A885-F61A29E0428D}" name="End"/>
+    <tableColumn id="3" xr3:uid="{D6295B2A-B818-864C-A5EA-D02EA76F9CB4}" name="Activity"/>
+    <tableColumn id="4" xr3:uid="{33236412-F754-E04E-84A6-91EAEF0494F1}" name="Comment"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2567BDC0-A04E-5C4C-9AAA-4EA175B1283D}" name="Table1" displayName="Table1" ref="A1:D135" totalsRowShown="0">
   <autoFilter ref="A1:D135" xr:uid="{92650681-87AE-8843-B8AE-73B4F45498A6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{55D453C5-1F86-C540-A3D0-A77F75750115}" name="Start" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{55D453C5-1F86-C540-A3D0-A77F75750115}" name="Start" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{9BA030C4-3502-B04E-A7B4-D67CDCE1CA4A}" name="End"/>
     <tableColumn id="3" xr3:uid="{2DCF4665-43E4-8447-9BD7-E4199779D3F7}" name="Activity"/>
     <tableColumn id="4" xr3:uid="{F2A2E482-4E7A-E74E-87D6-3481CC8E6ECA}" name="Comment"/>
@@ -833,29 +969,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BBD169-48D2-8F48-8801-52F9E2F03988}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -880,7 +1017,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -891,84 +1028,84 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+      <c r="A5" s="11">
         <v>43474.541666666664</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>43474.459027777775</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
-        <v>43474.459027777775</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <v>43474.500694444447</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="14">
-        <v>43474.500694444447</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>43474.646527777775</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
-        <v>43474.646527777775</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
+        <v>43474.730555555558</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
-        <v>43474.730555555558</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>43474.824305555558</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15">
-        <v>43474.824305555558</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>43474.825694444444</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15">
-        <v>43474.825694444444</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -992,7 +1129,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1003,7 +1140,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1014,22 +1151,22 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="14">
+      <c r="A16" s="11">
         <v>43475.885416666664</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14">
+      <c r="A17" s="11">
         <v>43476.158333333333</v>
       </c>
       <c r="C17" t="s">
@@ -1040,18 +1177,18 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="14">
+      <c r="A18" s="11">
         <v>43476.340277777781</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="14">
+      <c r="A19" s="11">
         <v>43475.972222222219</v>
       </c>
       <c r="B19" s="1">
@@ -1069,18 +1206,18 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
+        <v>43476.381944444445</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14">
-        <v>43476.381944444445</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1091,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1102,7 +1239,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1124,7 +1261,7 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1135,7 +1272,7 @@
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1182,7 +1319,7 @@
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1193,7 +1330,7 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1204,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1248,7 +1385,7 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1270,7 +1407,7 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1336,7 +1473,7 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1369,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1380,7 +1517,7 @@
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1435,11 +1572,608 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>43481.552083333336</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>43481.770833333336</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>43481.9375</v>
+      </c>
+      <c r="B56" s="1">
+        <v>43482.229166666664</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>43481.916666666664</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>43482.166666666664</v>
+      </c>
+      <c r="C58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>43482.120138888888</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>43482.253472222219</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>43482.361111111109</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>43482.333333333336</v>
+      </c>
+      <c r="B62" s="1">
+        <v>43482.354166666664</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>43482.506944444445</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>43482.59375</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>43482.770833333336</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>43482.8125</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>43482.895833333336</v>
+      </c>
+      <c r="C67" t="s">
+        <v>111</v>
+      </c>
+      <c r="D67" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>43482.9375</v>
+      </c>
+      <c r="B68" s="1">
+        <v>43483.208333333336</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>43483.074305555558</v>
+      </c>
+      <c r="C69" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>43483.188888888886</v>
+      </c>
+      <c r="C70" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>43483.25</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>43483.354166666664</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>43483.552083333336</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>43483.729166666664</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>43483.770833333336</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>43483.916666666664</v>
+      </c>
+      <c r="B76" s="1">
+        <v>43484.25</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>43484.142361111109</v>
+      </c>
+      <c r="C77" t="s">
+        <v>30</v>
+      </c>
+      <c r="D77" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>43484.191666666666</v>
+      </c>
+      <c r="C78" t="s">
+        <v>30</v>
+      </c>
+      <c r="D78" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>43484.291666666664</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>43484.354166666664</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>43484.611111111109</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>43484.8125</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>43484.916666666664</v>
+      </c>
+      <c r="B83" s="1">
+        <v>43485.25</v>
+      </c>
+      <c r="C83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>43485.3125</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>43485.520833333336</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>43485.59375</v>
+      </c>
+      <c r="B86" s="1">
+        <v>43485.625</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>43485.652083333334</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>43485.770833333336</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>43485.8125</v>
+      </c>
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>43485.9375</v>
+      </c>
+      <c r="B90" s="1">
+        <v>43486.25</v>
+      </c>
+      <c r="C90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>43486.270833333336</v>
+      </c>
+      <c r="C91" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>43486.184027777781</v>
+      </c>
+      <c r="C92" t="s">
+        <v>30</v>
+      </c>
+      <c r="D92" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>43486.84652777778</v>
+      </c>
+      <c r="C93" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>43486.9375</v>
+      </c>
+      <c r="B94" s="1">
+        <v>43487.229166666664</v>
+      </c>
+      <c r="C94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>43487.105555555558</v>
+      </c>
+      <c r="C95" t="s">
+        <v>30</v>
+      </c>
+      <c r="D95" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>43486.76458333333</v>
+      </c>
+      <c r="C96" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>43486.647222222222</v>
+      </c>
+      <c r="C97" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>43486.510416666664</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>43487.25</v>
+      </c>
+      <c r="C99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>43487.395833333336</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>43487.510416666664</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>43487.734722222223</v>
+      </c>
+      <c r="C102" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>43487.774305555555</v>
+      </c>
+      <c r="C103" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>43487.896527777775</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+      <c r="D104" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>43487.916666666664</v>
+      </c>
+      <c r="B105" s="1">
+        <v>43488.270833333336</v>
+      </c>
+      <c r="C105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>43488.28125</v>
+      </c>
+      <c r="C106" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>43488.388888888891</v>
+      </c>
+      <c r="C107" t="s">
+        <v>4</v>
+      </c>
+      <c r="D107" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1447,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D25C31-5891-F344-AFA8-EA292900C63D}">
   <dimension ref="A1:D135"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1637,7 +2371,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1756,7 +2490,7 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2278,7 +3012,7 @@
         <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2333,7 +3067,7 @@
         <v>4</v>
       </c>
       <c r="D75" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2388,7 +3122,7 @@
         <v>4</v>
       </c>
       <c r="D80" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2399,7 +3133,7 @@
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2410,7 +3144,7 @@
         <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2421,7 +3155,7 @@
         <v>4</v>
       </c>
       <c r="D83" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2465,7 +3199,7 @@
         <v>4</v>
       </c>
       <c r="D87" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2501,7 +3235,7 @@
         <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2523,7 +3257,7 @@
         <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2534,7 +3268,7 @@
         <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2545,7 +3279,7 @@
         <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2623,7 +3357,7 @@
         <v>4</v>
       </c>
       <c r="D101" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2649,7 +3383,7 @@
         <v>4</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2660,7 +3394,7 @@
         <v>4</v>
       </c>
       <c r="D104" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2685,7 +3419,7 @@
         <v>4</v>
       </c>
       <c r="D106" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2696,7 +3430,7 @@
         <v>4</v>
       </c>
       <c r="D107" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2762,7 +3496,7 @@
         <v>4</v>
       </c>
       <c r="D113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2773,7 +3507,7 @@
         <v>4</v>
       </c>
       <c r="D114" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2784,7 +3518,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2795,7 +3529,7 @@
         <v>4</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -2806,7 +3540,7 @@
         <v>4</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -2817,7 +3551,7 @@
         <v>4</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -2850,7 +3584,7 @@
         <v>4</v>
       </c>
       <c r="D121" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -2861,7 +3595,7 @@
         <v>4</v>
       </c>
       <c r="D122" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -2872,7 +3606,7 @@
         <v>4</v>
       </c>
       <c r="D123" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -2883,7 +3617,7 @@
         <v>4</v>
       </c>
       <c r="D124" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -2949,7 +3683,7 @@
         <v>4</v>
       </c>
       <c r="D130" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -2971,7 +3705,7 @@
         <v>4</v>
       </c>
       <c r="D132" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -2982,7 +3716,7 @@
         <v>4</v>
       </c>
       <c r="D133" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -3004,7 +3738,7 @@
         <v>4</v>
       </c>
       <c r="D135" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>